<commit_message>
Report Sale Order Line
</commit_message>
<xml_diff>
--- a/excel_import_export_demo/report_sale_order/report_sale_order_line.xlsx
+++ b/excel_import_export_demo/report_sale_order/report_sale_order_line.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Sale Order Report</t>
   </si>
@@ -43,6 +43,21 @@
   </si>
   <si>
     <t>Product</t>
+  </si>
+  <si>
+    <t>Sequence</t>
+  </si>
+  <si>
+    <t>Order Date</t>
+  </si>
+  <si>
+    <t>Product Code</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -476,53 +491,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMK6"/>
+  <dimension ref="A1:AMN6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
-    <col min="6" max="1026" width="11.5703125"/>
+    <col min="1" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
+    <col min="6" max="8" width="20.5703125" customWidth="1"/>
+    <col min="9" max="11" width="24.42578125" customWidth="1"/>
+    <col min="12" max="1029" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1025" ht="19.899999999999999" customHeight="1">
+    <row r="1" spans="1:1028" ht="19.899999999999999" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:1025">
+    <row r="2" spans="1:1028">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="2"/>
     </row>
-    <row r="4" spans="1:1025" s="4" customFormat="1">
+    <row r="4" spans="1:1028" s="4" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="ALV4"/>
-      <c r="ALW4"/>
-      <c r="ALX4"/>
       <c r="ALY4"/>
       <c r="ALZ4"/>
       <c r="AMA4"/>
@@ -536,11 +566,14 @@
       <c r="AMI4"/>
       <c r="AMJ4"/>
       <c r="AMK4"/>
+      <c r="AML4"/>
+      <c r="AMM4"/>
+      <c r="AMN4"/>
     </row>
-    <row r="6" spans="1:1025">
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+    <row r="6" spans="1:1028">
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
Report Sale Line Excel
</commit_message>
<xml_diff>
--- a/excel_import_export_demo/report_sale_order/report_sale_order_line.xlsx
+++ b/excel_import_export_demo/report_sale_order/report_sale_order_line.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Sale Order Report</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>Order Status</t>
+  </si>
+  <si>
+    <t>Invoice Status</t>
   </si>
 </sst>
 </file>
@@ -491,35 +497,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMN6"/>
+  <dimension ref="A1:AMP6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1"/>
-    <col min="6" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="11" width="24.42578125" customWidth="1"/>
-    <col min="12" max="1029" width="11.5703125"/>
+    <col min="3" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="8" max="10" width="20.5703125" customWidth="1"/>
+    <col min="11" max="13" width="24.42578125" customWidth="1"/>
+    <col min="14" max="1031" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1028" ht="19.899999999999999" customHeight="1">
+    <row r="1" spans="1:1030" ht="19.899999999999999" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:1028">
+    <row r="2" spans="1:1030">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="4" spans="1:1028" s="4" customFormat="1">
+    <row r="4" spans="1:1030" s="4" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -533,28 +539,32 @@
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="ALY4"/>
-      <c r="ALZ4"/>
       <c r="AMA4"/>
       <c r="AMB4"/>
       <c r="AMC4"/>
@@ -569,11 +579,13 @@
       <c r="AML4"/>
       <c r="AMM4"/>
       <c r="AMN4"/>
+      <c r="AMO4"/>
+      <c r="AMP4"/>
     </row>
-    <row r="6" spans="1:1028">
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+    <row r="6" spans="1:1030">
       <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>